<commit_message>
working midi. started waveshaping
</commit_message>
<xml_diff>
--- a/docs/TABLES.xlsx
+++ b/docs/TABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\27849\Documents\Stellenbosch\4\Skripsie\repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711C5BB5-C335-4247-B2AC-18DC070C7BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C3BE31-54D8-4F37-AFD8-D321CD347DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{13F9E6EA-CA08-4F40-B16C-1DEBF82AB9A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{13F9E6EA-CA08-4F40-B16C-1DEBF82AB9A5}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="343">
   <si>
     <t>fs</t>
   </si>
@@ -1087,6 +1087,12 @@
   </si>
   <si>
     <t>floor(harm/4)</t>
+  </si>
+  <si>
+    <t>time per sample</t>
+  </si>
+  <si>
+    <t>us</t>
   </si>
 </sst>
 </file>
@@ -17485,7 +17491,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="e">
-        <f t="shared" ref="D3:D66" si="2">MAX(0,_xlfn.FLOOR.MATH(LOG(C3,2))) + 2</f>
+        <f t="shared" ref="D3:D4" si="2">MAX(0,_xlfn.FLOOR.MATH(LOG(C3,2))) + 2</f>
         <v>#NUM!</v>
       </c>
       <c r="E3" t="e">
@@ -23594,8 +23600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A03B91-846E-4283-A9B8-522514C80769}">
   <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="O129" sqref="O127:O129"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P129" sqref="P129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32967,8 +32973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFF23AD-107D-4680-84B0-1579549AA9EA}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42196,45 +42202,46 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFC8783-4317-45FF-BE7A-6B58C4521927}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="11" width="16.42578125" customWidth="1"/>
+    <col min="7" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="12" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -42252,27 +42259,31 @@
         <v>907</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H12" si="1">_xlfn.FLOOR.MATH(G2/voices,1)</f>
+        <f>G2/F2</f>
+        <v>18.14</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I12" si="1">_xlfn.FLOOR.MATH(G2/voices,1)</f>
         <v>113</v>
       </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I12" si="2">FLOOR(H2/wtpervoice*wtp,1)</f>
+      <c r="J2">
+        <f t="shared" ref="J2:J12" si="2">FLOOR(I2/wtpervoice*wtp,1)</f>
         <v>11</v>
       </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J8" si="3">FLOOR(H2*adsrp,1)</f>
+      <c r="K2">
+        <f t="shared" ref="K2:K8" si="3">FLOOR(I2*adsrp,1)</f>
         <v>22</v>
       </c>
-      <c r="K2">
-        <f t="shared" ref="K2:K8" si="4">FLOOR(H2/2*filterp,1)</f>
+      <c r="L2">
+        <f t="shared" ref="L2:L8" si="4">FLOOR(I2/2*filterp,1)</f>
         <v>28</v>
       </c>
-      <c r="L2">
-        <f t="shared" ref="L2:L8" si="5">I2*wtpervoice+J2+2*K2</f>
+      <c r="M2">
+        <f t="shared" ref="M2:M8" si="5">J2*wtpervoice+K2+2*L2</f>
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -42291,27 +42302,31 @@
         <v>1814</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H12" si="6">G3/F3</f>
+        <v>18.14</v>
+      </c>
+      <c r="I3">
         <f t="shared" si="1"/>
         <v>226</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f t="shared" si="5"/>
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -42323,7 +42338,7 @@
         <v>193</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F12" si="6">F3+50</f>
+        <f t="shared" ref="F4:F12" si="7">F3+50</f>
         <v>150</v>
       </c>
       <c r="G4">
@@ -42331,27 +42346,31 @@
         <v>2721</v>
       </c>
       <c r="H4">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f t="shared" si="4"/>
         <v>85</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f t="shared" si="5"/>
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -42359,7 +42378,7 @@
         <v>8</v>
       </c>
       <c r="F5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="G5">
@@ -42367,27 +42386,31 @@
         <v>3628</v>
       </c>
       <c r="H5">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="1"/>
         <v>453</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f t="shared" si="4"/>
         <v>113</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="5"/>
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -42398,7 +42421,7 @@
         <v>206</v>
       </c>
       <c r="F6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
       <c r="G6">
@@ -42406,27 +42429,31 @@
         <v>4535</v>
       </c>
       <c r="H6">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="1"/>
         <v>566</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f t="shared" si="4"/>
         <v>141</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="5"/>
         <v>563</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -42435,7 +42462,7 @@
         <v>24</v>
       </c>
       <c r="F7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="G7">
@@ -42443,27 +42470,31 @@
         <v>5442</v>
       </c>
       <c r="H7">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="1"/>
         <v>680</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="3"/>
         <v>136</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f t="shared" si="4"/>
         <v>170</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="5"/>
         <v>680</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -42471,7 +42502,7 @@
         <v>0.3</v>
       </c>
       <c r="F8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>350</v>
       </c>
       <c r="G8">
@@ -42479,27 +42510,31 @@
         <v>6349</v>
       </c>
       <c r="H8">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="1"/>
         <v>793</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="3"/>
         <v>158</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f t="shared" si="4"/>
         <v>198</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="5"/>
         <v>791</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>200</v>
       </c>
@@ -42507,7 +42542,7 @@
         <v>0.2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>400</v>
       </c>
       <c r="G9">
@@ -42515,27 +42550,31 @@
         <v>7256</v>
       </c>
       <c r="H9">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="1"/>
         <v>907</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="J9">
-        <f>FLOOR(H9*adsrp,1)</f>
+      <c r="K9">
+        <f>FLOOR(I9*adsrp,1)</f>
         <v>181</v>
       </c>
-      <c r="K9">
-        <f>FLOOR(H9/2*filterp,1)</f>
+      <c r="L9">
+        <f>FLOOR(I9/2*filterp,1)</f>
         <v>226</v>
       </c>
-      <c r="L9">
-        <f>I9*wtpervoice+J9+2*K9</f>
+      <c r="M9">
+        <f>J9*wtpervoice+K9+2*L9</f>
         <v>903</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>202</v>
       </c>
@@ -42543,7 +42582,7 @@
         <v>0.5</v>
       </c>
       <c r="F10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>450</v>
       </c>
       <c r="G10">
@@ -42551,29 +42590,43 @@
         <v>8163</v>
       </c>
       <c r="H10">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
-      <c r="J10">
-        <f>FLOOR(H10*adsrp,1)</f>
+      <c r="K10">
+        <f>FLOOR(I10*adsrp,1)</f>
         <v>204</v>
       </c>
-      <c r="K10">
-        <f>FLOOR(H10/2*filterp,1)</f>
+      <c r="L10">
+        <f>FLOOR(I10/2*filterp,1)</f>
         <v>255</v>
       </c>
-      <c r="L10">
-        <f>I10*wtpervoice+J10+2*K10</f>
+      <c r="M10">
+        <f>J10*wtpervoice+K10+2*L10</f>
         <v>1020</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>341</v>
+      </c>
+      <c r="B11">
+        <f>1/fs * samplep * 1000000</f>
+        <v>18.140589569160998</v>
+      </c>
+      <c r="C11" t="s">
+        <v>342</v>
+      </c>
       <c r="F11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
       <c r="G11">
@@ -42581,29 +42634,33 @@
         <v>9070</v>
       </c>
       <c r="H11">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>1133</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f t="shared" si="2"/>
         <v>113</v>
       </c>
-      <c r="J11">
-        <f>FLOOR(H11*adsrp,1)</f>
+      <c r="K11">
+        <f>FLOOR(I11*adsrp,1)</f>
         <v>226</v>
       </c>
-      <c r="K11">
-        <f>FLOOR(H11/2*filterp,1)</f>
+      <c r="L11">
+        <f>FLOOR(I11/2*filterp,1)</f>
         <v>283</v>
       </c>
-      <c r="L11">
-        <f>I11*wtpervoice+J11+2*K11</f>
+      <c r="M11">
+        <f>J11*wtpervoice+K11+2*L11</f>
         <v>1131</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>550</v>
       </c>
       <c r="G12">
@@ -42611,23 +42668,27 @@
         <v>9977</v>
       </c>
       <c r="H12">
+        <f t="shared" si="6"/>
+        <v>18.14</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>1247</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="2"/>
         <v>124</v>
       </c>
-      <c r="J12">
-        <f>FLOOR(H12*adsrp,1)</f>
+      <c r="K12">
+        <f>FLOOR(I12*adsrp,1)</f>
         <v>249</v>
       </c>
-      <c r="K12">
-        <f>FLOOR(H12/2*filterp,1)</f>
+      <c r="L12">
+        <f>FLOOR(I12/2*filterp,1)</f>
         <v>311</v>
       </c>
-      <c r="L12">
-        <f>I12*wtpervoice+J12+2*K12</f>
+      <c r="M12">
+        <f>J12*wtpervoice+K12+2*L12</f>
         <v>1243</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more testing and diagrams
</commit_message>
<xml_diff>
--- a/docs/TABLES.xlsx
+++ b/docs/TABLES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\27849\Documents\Stellenbosch\4\Skripsie\repo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C3BE31-54D8-4F37-AFD8-D321CD347DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A761E-A026-430F-B979-42A8C1FA19BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{13F9E6EA-CA08-4F40-B16C-1DEBF82AB9A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{13F9E6EA-CA08-4F40-B16C-1DEBF82AB9A5}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet name="notes float" sheetId="9" r:id="rId3"/>
     <sheet name="tanh" sheetId="8" r:id="rId4"/>
     <sheet name="fpu instr set" sheetId="10" r:id="rId5"/>
-    <sheet name="trig buffer" sheetId="6" r:id="rId6"/>
-    <sheet name="cycles" sheetId="5" r:id="rId7"/>
-    <sheet name="lpf" sheetId="7" r:id="rId8"/>
-    <sheet name="Notes def" sheetId="4" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId10"/>
-    <sheet name="ADSR" sheetId="2" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId6"/>
+    <sheet name="trig buffer" sheetId="6" r:id="rId7"/>
+    <sheet name="cycles" sheetId="5" r:id="rId8"/>
+    <sheet name="lpf" sheetId="7" r:id="rId9"/>
+    <sheet name="Notes def" sheetId="4" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId11"/>
+    <sheet name="ADSR" sheetId="2" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="a">ADSR!$B$3</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="345">
   <si>
     <t>fs</t>
   </si>
@@ -1094,6 +1095,12 @@
   <si>
     <t>us</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
 </sst>
 </file>
 
@@ -1122,7 +1129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1130,17 +1137,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13685,6 +13710,1422 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653818A3-EE68-413B-B9A3-E0133145B671}">
+  <dimension ref="A1:C129"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="str">
+        <f>"#define " &amp; B23 &amp; " " &amp;A23</f>
+        <v>#define A0 21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" ref="C24:C87" si="0">"#define " &amp; B24 &amp; " " &amp;A24</f>
+        <v>#define As0_Bb0 22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#define B0 23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#define C1 24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Cs1_Db1 25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#define D1 26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Ds1_Eb1 27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#define E1 28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#define F1 29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Fs1_Gb1 30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>#define G1 31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Gs1_Ab1 32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>#define A1 33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>#define As1_Bb1 34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>#define B1 35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>#define C2 36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Cs2_Db2 37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>#define D2 38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Ds2_Eb2 39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>#define E2 40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>#define F2 41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Fs2_Gb2 42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>#define G2 43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Gs2_Ab2 44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>#define A2 45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>#define As2_Bb2 46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>#define B2 47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>#define C3 48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Cs3_Db3 49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>#define D3 50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Ds3_Eb3 51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>#define E3 52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>#define F3 53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Fs3_Gb3 54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>#define G3 55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Gs3_Ab3 56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>#define A3 57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>#define As3_Bb3 58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>#define B3 59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>#define C4 60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>159</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Cs4_Db4 61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>#define D4 62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Ds4_Eb4 63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>#define E4 64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="0"/>
+        <v>#define F4 65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Fs4_Gb4 66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="0"/>
+        <v>#define G4 67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Gs4_Ab4 68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>142</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="0"/>
+        <v>#define A4 69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="0"/>
+        <v>#define As4_Bb4 70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="0"/>
+        <v>#define B4 71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="0"/>
+        <v>#define C5 72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Cs5_Db5 73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="0"/>
+        <v>#define D5 74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Ds5_Eb5 75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>57</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="0"/>
+        <v>#define E5 76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="0"/>
+        <v>#define F5 77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Fs5_Gb5 78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="0"/>
+        <v>#define G5 79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>167</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Gs5_Ab5 80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="0"/>
+        <v>#define A5 81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="0"/>
+        <v>#define As5_Bb5 82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="0"/>
+        <v>#define B5 83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>49</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="0"/>
+        <v>#define C6 84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>169</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="0"/>
+        <v>#define Cs6_Db6 85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>47</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" ref="C88:C129" si="1">"#define " &amp; B88 &amp; " " &amp;A88</f>
+        <v>#define D6 86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>170</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Ds6_Eb6 87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>#define E6 88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="1"/>
+        <v>#define F6 89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>171</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Fs6_Gb6 90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>42</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="1"/>
+        <v>#define G6 91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Gs6_Ab6 92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="1"/>
+        <v>#define A6 93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="1"/>
+        <v>#define As6_Bb6 94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="1"/>
+        <v>#define B6 95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>37</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="1"/>
+        <v>#define C7 96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>174</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Cs7_Db7 97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>35</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="1"/>
+        <v>#define D7 98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>175</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Ds7_Eb7 99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>33</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="1"/>
+        <v>#define E7 100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>32</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="1"/>
+        <v>#define F7 101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>176</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Fs7_Gb7 102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>30</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="1"/>
+        <v>#define G7 103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>177</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Gs7_Ab7 104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>28</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="1"/>
+        <v>#define A7 105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>178</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="1"/>
+        <v>#define As7_Bb7 106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>26</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="1"/>
+        <v>#define B7 107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>25</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="1"/>
+        <v>#define C8 108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>179</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Cs8_Db8 109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>23</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="1"/>
+        <v>#define D8 110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>180</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Ds8_Eb8 111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>21</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="1"/>
+        <v>#define E8 112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="1"/>
+        <v>#define F8 113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>181</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Fs8_Gb8 114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>18</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="1"/>
+        <v>#define G8 115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>182</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Gs8_Ab8 116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>16</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="1"/>
+        <v>#define A8 117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>183</v>
+      </c>
+      <c r="C120" t="str">
+        <f t="shared" si="1"/>
+        <v>#define As8_Bb8 118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121" t="str">
+        <f t="shared" si="1"/>
+        <v>#define B8 119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>13</v>
+      </c>
+      <c r="C122" t="str">
+        <f t="shared" si="1"/>
+        <v>#define C9 120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>184</v>
+      </c>
+      <c r="C123" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Cs9_Db9 121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" t="str">
+        <f t="shared" si="1"/>
+        <v>#define D9 122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>185</v>
+      </c>
+      <c r="C125" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Ds9_Eb9 123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" t="str">
+        <f t="shared" si="1"/>
+        <v>#define E9 124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="1"/>
+        <v>#define F9 125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>186</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="1"/>
+        <v>#define Fs9_Gb9 126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129" t="str">
+        <f t="shared" si="1"/>
+        <v>#define G9 127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE282B9-77DE-44DD-A650-D1B2E3BEDB6C}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -13786,7 +15227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F294FAD-4759-400C-8C67-4D0D2DB61129}">
   <dimension ref="A1:G257"/>
   <sheetViews>
@@ -23600,8 +25041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A03B91-846E-4283-A9B8-522514C80769}">
   <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P129" sqref="P129"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:P129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32973,8 +34414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFF23AD-107D-4680-84B0-1579549AA9EA}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33451,6 +34892,52 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F083BC-AEF4-4BCD-B7AA-11F7F8456533}">
+  <dimension ref="B5:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="9" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDFE157-4BDB-419F-A0D7-D50F51A56394}">
   <dimension ref="A1:I263"/>
   <sheetViews>
@@ -42200,11 +43687,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFC8783-4317-45FF-BE7A-6B58C4521927}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -42697,7 +44184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B90420-666B-4F7F-A94A-9EF0CD4851BA}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -42881,1420 +44368,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653818A3-EE68-413B-B9A3-E0133145B671}">
-  <dimension ref="A1:C129"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" t="str">
-        <f>"#define " &amp; B23 &amp; " " &amp;A23</f>
-        <v>#define A0 21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" ref="C24:C87" si="0">"#define " &amp; B24 &amp; " " &amp;A24</f>
-        <v>#define As0_Bb0 22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>#define B0 23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>#define C1 24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>144</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Cs1_Db1 25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>#define D1 26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Ds1_Eb1 27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>#define E1 28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>#define F1 29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Fs1_Gb1 30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>#define G1 31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Gs1_Ab1 32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" t="str">
-        <f t="shared" si="0"/>
-        <v>#define A1 33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" t="str">
-        <f t="shared" si="0"/>
-        <v>#define As1_Bb1 34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" t="str">
-        <f t="shared" si="0"/>
-        <v>#define B1 35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" t="str">
-        <f t="shared" si="0"/>
-        <v>#define C2 36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>149</v>
-      </c>
-      <c r="C39" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Cs2_Db2 37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" t="str">
-        <f t="shared" si="0"/>
-        <v>#define D2 38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C41" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Ds2_Eb2 39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" t="str">
-        <f t="shared" si="0"/>
-        <v>#define E2 40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" t="str">
-        <f t="shared" si="0"/>
-        <v>#define F2 41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>151</v>
-      </c>
-      <c r="C44" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Fs2_Gb2 42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" t="str">
-        <f t="shared" si="0"/>
-        <v>#define G2 43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>152</v>
-      </c>
-      <c r="C46" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Gs2_Ab2 44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" t="str">
-        <f t="shared" si="0"/>
-        <v>#define A2 45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>153</v>
-      </c>
-      <c r="C48" t="str">
-        <f t="shared" si="0"/>
-        <v>#define As2_Bb2 46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" t="str">
-        <f t="shared" si="0"/>
-        <v>#define B2 47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" t="str">
-        <f t="shared" si="0"/>
-        <v>#define C3 48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
-        <v>154</v>
-      </c>
-      <c r="C51" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Cs3_Db3 49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
-        <v>84</v>
-      </c>
-      <c r="C52" t="str">
-        <f t="shared" si="0"/>
-        <v>#define D3 50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Ds3_Eb3 51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" t="str">
-        <f t="shared" si="0"/>
-        <v>#define E3 52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" t="str">
-        <f t="shared" si="0"/>
-        <v>#define F3 53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>156</v>
-      </c>
-      <c r="C56" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Fs3_Gb3 54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>79</v>
-      </c>
-      <c r="C57" t="str">
-        <f t="shared" si="0"/>
-        <v>#define G3 55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>157</v>
-      </c>
-      <c r="C58" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Gs3_Ab3 56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" t="str">
-        <f t="shared" si="0"/>
-        <v>#define A3 57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>158</v>
-      </c>
-      <c r="C60" t="str">
-        <f t="shared" si="0"/>
-        <v>#define As3_Bb3 58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>74</v>
-      </c>
-      <c r="C61" t="str">
-        <f t="shared" si="0"/>
-        <v>#define B3 59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
-        <v>187</v>
-      </c>
-      <c r="C62" t="str">
-        <f t="shared" si="0"/>
-        <v>#define C4 60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>159</v>
-      </c>
-      <c r="C63" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Cs4_Db4 61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" t="str">
-        <f t="shared" si="0"/>
-        <v>#define D4 62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>160</v>
-      </c>
-      <c r="C65" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Ds4_Eb4 63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" t="str">
-        <f t="shared" si="0"/>
-        <v>#define E4 64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>65</v>
-      </c>
-      <c r="B67" t="s">
-        <v>68</v>
-      </c>
-      <c r="C67" t="str">
-        <f t="shared" si="0"/>
-        <v>#define F4 65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>66</v>
-      </c>
-      <c r="B68" t="s">
-        <v>161</v>
-      </c>
-      <c r="C68" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Fs4_Gb4 66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>67</v>
-      </c>
-      <c r="B69" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" t="str">
-        <f t="shared" si="0"/>
-        <v>#define G4 67</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>68</v>
-      </c>
-      <c r="B70" t="s">
-        <v>162</v>
-      </c>
-      <c r="C70" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Gs4_Ab4 68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>69</v>
-      </c>
-      <c r="B71" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" t="str">
-        <f t="shared" si="0"/>
-        <v>#define A4 69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>70</v>
-      </c>
-      <c r="B72" t="s">
-        <v>163</v>
-      </c>
-      <c r="C72" t="str">
-        <f t="shared" si="0"/>
-        <v>#define As4_Bb4 70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>71</v>
-      </c>
-      <c r="B73" t="s">
-        <v>62</v>
-      </c>
-      <c r="C73" t="str">
-        <f t="shared" si="0"/>
-        <v>#define B4 71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>72</v>
-      </c>
-      <c r="B74" t="s">
-        <v>61</v>
-      </c>
-      <c r="C74" t="str">
-        <f t="shared" si="0"/>
-        <v>#define C5 72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>164</v>
-      </c>
-      <c r="C75" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Cs5_Db5 73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>74</v>
-      </c>
-      <c r="B76" t="s">
-        <v>59</v>
-      </c>
-      <c r="C76" t="str">
-        <f t="shared" si="0"/>
-        <v>#define D5 74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>75</v>
-      </c>
-      <c r="B77" t="s">
-        <v>165</v>
-      </c>
-      <c r="C77" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Ds5_Eb5 75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>76</v>
-      </c>
-      <c r="B78" t="s">
-        <v>57</v>
-      </c>
-      <c r="C78" t="str">
-        <f t="shared" si="0"/>
-        <v>#define E5 76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>77</v>
-      </c>
-      <c r="B79" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" t="str">
-        <f t="shared" si="0"/>
-        <v>#define F5 77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>78</v>
-      </c>
-      <c r="B80" t="s">
-        <v>166</v>
-      </c>
-      <c r="C80" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Fs5_Gb5 78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>79</v>
-      </c>
-      <c r="B81" t="s">
-        <v>54</v>
-      </c>
-      <c r="C81" t="str">
-        <f t="shared" si="0"/>
-        <v>#define G5 79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>80</v>
-      </c>
-      <c r="B82" t="s">
-        <v>167</v>
-      </c>
-      <c r="C82" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Gs5_Ab5 80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>81</v>
-      </c>
-      <c r="B83" t="s">
-        <v>52</v>
-      </c>
-      <c r="C83" t="str">
-        <f t="shared" si="0"/>
-        <v>#define A5 81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>82</v>
-      </c>
-      <c r="B84" t="s">
-        <v>168</v>
-      </c>
-      <c r="C84" t="str">
-        <f t="shared" si="0"/>
-        <v>#define As5_Bb5 82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>83</v>
-      </c>
-      <c r="B85" t="s">
-        <v>50</v>
-      </c>
-      <c r="C85" t="str">
-        <f t="shared" si="0"/>
-        <v>#define B5 83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>84</v>
-      </c>
-      <c r="B86" t="s">
-        <v>49</v>
-      </c>
-      <c r="C86" t="str">
-        <f t="shared" si="0"/>
-        <v>#define C6 84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>85</v>
-      </c>
-      <c r="B87" t="s">
-        <v>169</v>
-      </c>
-      <c r="C87" t="str">
-        <f t="shared" si="0"/>
-        <v>#define Cs6_Db6 85</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>86</v>
-      </c>
-      <c r="B88" t="s">
-        <v>47</v>
-      </c>
-      <c r="C88" t="str">
-        <f t="shared" ref="C88:C129" si="1">"#define " &amp; B88 &amp; " " &amp;A88</f>
-        <v>#define D6 86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>87</v>
-      </c>
-      <c r="B89" t="s">
-        <v>170</v>
-      </c>
-      <c r="C89" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Ds6_Eb6 87</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>88</v>
-      </c>
-      <c r="B90" t="s">
-        <v>45</v>
-      </c>
-      <c r="C90" t="str">
-        <f t="shared" si="1"/>
-        <v>#define E6 88</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>89</v>
-      </c>
-      <c r="B91" t="s">
-        <v>44</v>
-      </c>
-      <c r="C91" t="str">
-        <f t="shared" si="1"/>
-        <v>#define F6 89</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>90</v>
-      </c>
-      <c r="B92" t="s">
-        <v>171</v>
-      </c>
-      <c r="C92" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Fs6_Gb6 90</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>91</v>
-      </c>
-      <c r="B93" t="s">
-        <v>42</v>
-      </c>
-      <c r="C93" t="str">
-        <f t="shared" si="1"/>
-        <v>#define G6 91</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>92</v>
-      </c>
-      <c r="B94" t="s">
-        <v>172</v>
-      </c>
-      <c r="C94" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Gs6_Ab6 92</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>93</v>
-      </c>
-      <c r="B95" t="s">
-        <v>40</v>
-      </c>
-      <c r="C95" t="str">
-        <f t="shared" si="1"/>
-        <v>#define A6 93</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>94</v>
-      </c>
-      <c r="B96" t="s">
-        <v>173</v>
-      </c>
-      <c r="C96" t="str">
-        <f t="shared" si="1"/>
-        <v>#define As6_Bb6 94</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>95</v>
-      </c>
-      <c r="B97" t="s">
-        <v>38</v>
-      </c>
-      <c r="C97" t="str">
-        <f t="shared" si="1"/>
-        <v>#define B6 95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>96</v>
-      </c>
-      <c r="B98" t="s">
-        <v>37</v>
-      </c>
-      <c r="C98" t="str">
-        <f t="shared" si="1"/>
-        <v>#define C7 96</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>97</v>
-      </c>
-      <c r="B99" t="s">
-        <v>174</v>
-      </c>
-      <c r="C99" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Cs7_Db7 97</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>98</v>
-      </c>
-      <c r="B100" t="s">
-        <v>35</v>
-      </c>
-      <c r="C100" t="str">
-        <f t="shared" si="1"/>
-        <v>#define D7 98</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>99</v>
-      </c>
-      <c r="B101" t="s">
-        <v>175</v>
-      </c>
-      <c r="C101" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Ds7_Eb7 99</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>100</v>
-      </c>
-      <c r="B102" t="s">
-        <v>33</v>
-      </c>
-      <c r="C102" t="str">
-        <f t="shared" si="1"/>
-        <v>#define E7 100</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>101</v>
-      </c>
-      <c r="B103" t="s">
-        <v>32</v>
-      </c>
-      <c r="C103" t="str">
-        <f t="shared" si="1"/>
-        <v>#define F7 101</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>102</v>
-      </c>
-      <c r="B104" t="s">
-        <v>176</v>
-      </c>
-      <c r="C104" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Fs7_Gb7 102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>103</v>
-      </c>
-      <c r="B105" t="s">
-        <v>30</v>
-      </c>
-      <c r="C105" t="str">
-        <f t="shared" si="1"/>
-        <v>#define G7 103</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>104</v>
-      </c>
-      <c r="B106" t="s">
-        <v>177</v>
-      </c>
-      <c r="C106" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Gs7_Ab7 104</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>105</v>
-      </c>
-      <c r="B107" t="s">
-        <v>28</v>
-      </c>
-      <c r="C107" t="str">
-        <f t="shared" si="1"/>
-        <v>#define A7 105</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>106</v>
-      </c>
-      <c r="B108" t="s">
-        <v>178</v>
-      </c>
-      <c r="C108" t="str">
-        <f t="shared" si="1"/>
-        <v>#define As7_Bb7 106</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>107</v>
-      </c>
-      <c r="B109" t="s">
-        <v>26</v>
-      </c>
-      <c r="C109" t="str">
-        <f t="shared" si="1"/>
-        <v>#define B7 107</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>108</v>
-      </c>
-      <c r="B110" t="s">
-        <v>25</v>
-      </c>
-      <c r="C110" t="str">
-        <f t="shared" si="1"/>
-        <v>#define C8 108</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>109</v>
-      </c>
-      <c r="B111" t="s">
-        <v>179</v>
-      </c>
-      <c r="C111" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Cs8_Db8 109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>110</v>
-      </c>
-      <c r="B112" t="s">
-        <v>23</v>
-      </c>
-      <c r="C112" t="str">
-        <f t="shared" si="1"/>
-        <v>#define D8 110</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>111</v>
-      </c>
-      <c r="B113" t="s">
-        <v>180</v>
-      </c>
-      <c r="C113" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Ds8_Eb8 111</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>112</v>
-      </c>
-      <c r="B114" t="s">
-        <v>21</v>
-      </c>
-      <c r="C114" t="str">
-        <f t="shared" si="1"/>
-        <v>#define E8 112</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>113</v>
-      </c>
-      <c r="B115" t="s">
-        <v>20</v>
-      </c>
-      <c r="C115" t="str">
-        <f t="shared" si="1"/>
-        <v>#define F8 113</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>114</v>
-      </c>
-      <c r="B116" t="s">
-        <v>181</v>
-      </c>
-      <c r="C116" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Fs8_Gb8 114</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>115</v>
-      </c>
-      <c r="B117" t="s">
-        <v>18</v>
-      </c>
-      <c r="C117" t="str">
-        <f t="shared" si="1"/>
-        <v>#define G8 115</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>116</v>
-      </c>
-      <c r="B118" t="s">
-        <v>182</v>
-      </c>
-      <c r="C118" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Gs8_Ab8 116</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>117</v>
-      </c>
-      <c r="B119" t="s">
-        <v>16</v>
-      </c>
-      <c r="C119" t="str">
-        <f t="shared" si="1"/>
-        <v>#define A8 117</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>118</v>
-      </c>
-      <c r="B120" t="s">
-        <v>183</v>
-      </c>
-      <c r="C120" t="str">
-        <f t="shared" si="1"/>
-        <v>#define As8_Bb8 118</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>119</v>
-      </c>
-      <c r="B121" t="s">
-        <v>14</v>
-      </c>
-      <c r="C121" t="str">
-        <f t="shared" si="1"/>
-        <v>#define B8 119</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>120</v>
-      </c>
-      <c r="B122" t="s">
-        <v>13</v>
-      </c>
-      <c r="C122" t="str">
-        <f t="shared" si="1"/>
-        <v>#define C9 120</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>121</v>
-      </c>
-      <c r="B123" t="s">
-        <v>184</v>
-      </c>
-      <c r="C123" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Cs9_Db9 121</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>122</v>
-      </c>
-      <c r="B124" t="s">
-        <v>11</v>
-      </c>
-      <c r="C124" t="str">
-        <f t="shared" si="1"/>
-        <v>#define D9 122</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>123</v>
-      </c>
-      <c r="B125" t="s">
-        <v>185</v>
-      </c>
-      <c r="C125" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Ds9_Eb9 123</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>124</v>
-      </c>
-      <c r="B126" t="s">
-        <v>9</v>
-      </c>
-      <c r="C126" t="str">
-        <f t="shared" si="1"/>
-        <v>#define E9 124</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>125</v>
-      </c>
-      <c r="B127" t="s">
-        <v>8</v>
-      </c>
-      <c r="C127" t="str">
-        <f t="shared" si="1"/>
-        <v>#define F9 125</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128">
-        <v>126</v>
-      </c>
-      <c r="B128" t="s">
-        <v>186</v>
-      </c>
-      <c r="C128" t="str">
-        <f t="shared" si="1"/>
-        <v>#define Fs9_Gb9 126</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129">
-        <v>127</v>
-      </c>
-      <c r="B129" t="s">
-        <v>6</v>
-      </c>
-      <c r="C129" t="str">
-        <f t="shared" si="1"/>
-        <v>#define G9 127</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>